<commit_message>
update advisors and tablets
</commit_message>
<xml_diff>
--- a/boardgames/seafall/spoilers/advisors.xlsx
+++ b/boardgames/seafall/spoilers/advisors.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10513"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karhohs\Documents\GitHub\boardgame-bookie\boardgames\seafall\spoilers\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Kyle/Documents/GitHub/boardgame-bookie/boardgames/seafall/spoilers/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{ED87B58D-E0CE-1E41-BF37-20F140AEEC16}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20100" yWindow="4320" windowWidth="28800" windowHeight="17598" tabRatio="500"/>
+    <workbookView xWindow="320" yWindow="940" windowWidth="28800" windowHeight="17600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="advisors" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="172">
   <si>
     <t>name</t>
   </si>
@@ -531,12 +532,21 @@
   </si>
   <si>
     <t>empty_slots</t>
+  </si>
+  <si>
+    <t>society_rank</t>
+  </si>
+  <si>
+    <t>chart_to_end_of_world</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -847,17 +857,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q73"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:S73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="82" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P70" sqref="P70"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q41" sqref="Q41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="16" max="16" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -904,36 +918,42 @@
         <v>168</v>
       </c>
       <c r="P1" t="s">
+        <v>170</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>169</v>
+      </c>
+      <c r="R1" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>58</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -956,16 +976,19 @@
       <c r="O2">
         <v>1</v>
       </c>
-      <c r="P2">
-        <v>1</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.6">
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="S2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -974,13 +997,13 @@
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -995,10 +1018,10 @@
         <v>0</v>
       </c>
       <c r="K3">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="L3">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="M3" t="s">
         <v>17</v>
@@ -1007,36 +1030,39 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>2</v>
-      </c>
-      <c r="P3">
-        <v>1</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.6">
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <v>11</v>
+      </c>
+      <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="S3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D4" t="s">
         <v>16</v>
       </c>
       <c r="E4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -1060,30 +1086,33 @@
         <v>0</v>
       </c>
       <c r="O4">
-        <v>1</v>
-      </c>
-      <c r="P4">
-        <v>1</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.6">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>1</v>
+      </c>
+      <c r="S4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="E5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -1095,7 +1124,7 @@
         <v>0</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5">
         <v>0</v>
@@ -1113,36 +1142,39 @@
         <v>0</v>
       </c>
       <c r="O5">
-        <v>1</v>
-      </c>
-      <c r="P5">
-        <v>1</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.6">
+        <v>2</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>1</v>
+      </c>
+      <c r="S5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -1154,10 +1186,10 @@
         <v>0</v>
       </c>
       <c r="K6">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="L6">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="M6" t="s">
         <v>17</v>
@@ -1168,25 +1200,28 @@
       <c r="O6">
         <v>0</v>
       </c>
-      <c r="P6">
-        <v>1</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.6">
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>1</v>
+      </c>
+      <c r="S6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -1198,10 +1233,10 @@
         <v>0</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7">
         <v>0</v>
@@ -1210,7 +1245,7 @@
         <v>0</v>
       </c>
       <c r="L7">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="M7" t="s">
         <v>17</v>
@@ -1219,33 +1254,36 @@
         <v>0</v>
       </c>
       <c r="O7">
-        <v>2</v>
-      </c>
-      <c r="P7">
-        <v>1</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.6">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>1</v>
+      </c>
+      <c r="S7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -1260,10 +1298,10 @@
         <v>0</v>
       </c>
       <c r="K8">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="L8">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="M8" t="s">
         <v>17</v>
@@ -1272,24 +1310,30 @@
         <v>0</v>
       </c>
       <c r="O8">
-        <v>0</v>
-      </c>
-      <c r="P8">
-        <v>1</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.6">
+        <v>1</v>
+      </c>
+      <c r="P8" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q8">
+        <v>41</v>
+      </c>
+      <c r="R8">
+        <v>1</v>
+      </c>
+      <c r="S8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D9" t="s">
         <v>31</v>
@@ -1304,7 +1348,7 @@
         <v>0</v>
       </c>
       <c r="H9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I9">
         <v>0</v>
@@ -1313,10 +1357,10 @@
         <v>0</v>
       </c>
       <c r="K9">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="L9">
-        <v>-2</v>
+        <v>-4</v>
       </c>
       <c r="M9" t="s">
         <v>17</v>
@@ -1325,27 +1369,30 @@
         <v>0</v>
       </c>
       <c r="O9">
-        <v>0</v>
-      </c>
-      <c r="P9">
-        <v>1</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.6">
+        <v>1</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>1</v>
+      </c>
+      <c r="S9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -1360,16 +1407,16 @@
         <v>0</v>
       </c>
       <c r="I10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10">
         <v>0</v>
       </c>
       <c r="K10">
-        <v>-4</v>
+        <v>0</v>
       </c>
       <c r="L10">
-        <v>-4</v>
+        <v>0</v>
       </c>
       <c r="M10" t="s">
         <v>17</v>
@@ -1378,18 +1425,21 @@
         <v>0</v>
       </c>
       <c r="O10">
-        <v>1</v>
-      </c>
-      <c r="P10">
-        <v>1</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.6">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>1</v>
+      </c>
+      <c r="S10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -1431,33 +1481,36 @@
         <v>0</v>
       </c>
       <c r="O11">
-        <v>0</v>
-      </c>
-      <c r="P11">
-        <v>1</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.6">
+        <v>1</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>1</v>
+      </c>
+      <c r="S11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D12" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="E12">
         <v>0</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -1466,7 +1519,7 @@
         <v>0</v>
       </c>
       <c r="I12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J12">
         <v>0</v>
@@ -1484,27 +1537,30 @@
         <v>0</v>
       </c>
       <c r="O12">
-        <v>1</v>
-      </c>
-      <c r="P12">
-        <v>1</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.6">
+        <v>2</v>
+      </c>
+      <c r="Q12">
+        <v>24</v>
+      </c>
+      <c r="R12">
+        <v>1</v>
+      </c>
+      <c r="S12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -1513,10 +1569,10 @@
         <v>0</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I13">
         <v>0</v>
@@ -1525,10 +1581,10 @@
         <v>0</v>
       </c>
       <c r="K13">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="L13">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="M13" t="s">
         <v>17</v>
@@ -1537,18 +1593,21 @@
         <v>0</v>
       </c>
       <c r="O13">
-        <v>1</v>
-      </c>
-      <c r="P13">
-        <v>1</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.6">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>1</v>
+      </c>
+      <c r="S13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -1557,7 +1616,7 @@
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -1572,16 +1631,16 @@
         <v>0</v>
       </c>
       <c r="I14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J14">
         <v>0</v>
       </c>
       <c r="K14">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="L14">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="M14" t="s">
         <v>17</v>
@@ -1590,24 +1649,27 @@
         <v>0</v>
       </c>
       <c r="O14">
-        <v>2</v>
-      </c>
-      <c r="P14">
-        <v>1</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.6">
+        <v>1</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <v>1</v>
+      </c>
+      <c r="S14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D15" t="s">
         <v>28</v>
@@ -1625,7 +1687,7 @@
         <v>0</v>
       </c>
       <c r="I15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J15">
         <v>0</v>
@@ -1643,33 +1705,36 @@
         <v>0</v>
       </c>
       <c r="O15">
-        <v>0</v>
-      </c>
-      <c r="P15">
-        <v>1</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.6">
+        <v>2</v>
+      </c>
+      <c r="Q15">
+        <v>9</v>
+      </c>
+      <c r="R15">
+        <v>1</v>
+      </c>
+      <c r="S15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16">
         <v>0</v>
@@ -1684,10 +1749,10 @@
         <v>0</v>
       </c>
       <c r="K16">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="L16">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="M16" t="s">
         <v>17</v>
@@ -1698,16 +1763,19 @@
       <c r="O16">
         <v>1</v>
       </c>
-      <c r="P16">
-        <v>1</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.6">
+      <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <v>1</v>
+      </c>
+      <c r="S16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -1725,7 +1793,7 @@
         <v>0</v>
       </c>
       <c r="G17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H17">
         <v>2</v>
@@ -1749,16 +1817,19 @@
         <v>0</v>
       </c>
       <c r="O17">
-        <v>2</v>
-      </c>
-      <c r="P17">
-        <v>1</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.6">
+        <v>1</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <v>1</v>
+      </c>
+      <c r="S17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>52</v>
       </c>
@@ -1804,37 +1875,40 @@
       <c r="O18">
         <v>2</v>
       </c>
-      <c r="P18">
-        <v>1</v>
-      </c>
-      <c r="Q18" t="s">
+      <c r="Q18">
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <v>1</v>
+      </c>
+      <c r="S18" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.6">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>23</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D19" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F19">
         <v>0</v>
       </c>
       <c r="G19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I19">
         <v>0</v>
@@ -1857,22 +1931,25 @@
       <c r="O19">
         <v>1</v>
       </c>
-      <c r="P19">
-        <v>1</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.6">
+      <c r="Q19">
+        <v>0</v>
+      </c>
+      <c r="R19">
+        <v>1</v>
+      </c>
+      <c r="S19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D20" t="s">
         <v>50</v>
@@ -1884,10 +1961,10 @@
         <v>0</v>
       </c>
       <c r="G20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I20">
         <v>0</v>
@@ -1908,27 +1985,30 @@
         <v>0</v>
       </c>
       <c r="O20">
-        <v>0</v>
-      </c>
-      <c r="P20">
-        <v>1</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.6">
+        <v>2</v>
+      </c>
+      <c r="Q20">
+        <v>29</v>
+      </c>
+      <c r="R20">
+        <v>1</v>
+      </c>
+      <c r="S20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
       <c r="C21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="E21">
         <v>0</v>
@@ -1940,10 +2020,10 @@
         <v>0</v>
       </c>
       <c r="H21">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J21">
         <v>0</v>
@@ -1961,36 +2041,39 @@
         <v>0</v>
       </c>
       <c r="O21">
-        <v>1</v>
-      </c>
-      <c r="P21">
-        <v>1</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.6">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
+      <c r="R21">
+        <v>1</v>
+      </c>
+      <c r="S21" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
       <c r="C22">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="E22">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F22">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G22">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H22">
         <v>0</v>
@@ -2002,7 +2085,7 @@
         <v>0</v>
       </c>
       <c r="K22">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="L22">
         <v>0</v>
@@ -2016,28 +2099,31 @@
       <c r="O22">
         <v>0</v>
       </c>
-      <c r="P22">
-        <v>2</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.6">
+      <c r="Q22">
+        <v>0</v>
+      </c>
+      <c r="R22">
+        <v>2</v>
+      </c>
+      <c r="S22" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
       <c r="C23">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D23" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="E23">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F23">
         <v>0</v>
@@ -2058,7 +2144,7 @@
         <v>0</v>
       </c>
       <c r="L23">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="M23" t="s">
         <v>164</v>
@@ -2067,27 +2153,30 @@
         <v>0</v>
       </c>
       <c r="O23">
-        <v>2</v>
-      </c>
-      <c r="P23">
-        <v>2</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.6">
+        <v>1</v>
+      </c>
+      <c r="Q23">
+        <v>3</v>
+      </c>
+      <c r="R23">
+        <v>2</v>
+      </c>
+      <c r="S23" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
       <c r="C24">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D24" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E24">
         <v>0</v>
@@ -2096,19 +2185,19 @@
         <v>0</v>
       </c>
       <c r="G24">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H24">
         <v>0</v>
       </c>
       <c r="I24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J24">
         <v>0</v>
       </c>
       <c r="K24">
-        <v>-4</v>
+        <v>0</v>
       </c>
       <c r="L24">
         <v>0</v>
@@ -2120,27 +2209,30 @@
         <v>0</v>
       </c>
       <c r="O24">
-        <v>0</v>
-      </c>
-      <c r="P24">
-        <v>2</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.6">
+        <v>1</v>
+      </c>
+      <c r="Q24">
+        <v>0</v>
+      </c>
+      <c r="R24">
+        <v>2</v>
+      </c>
+      <c r="S24" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="B25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C25">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D25" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -2149,10 +2241,10 @@
         <v>0</v>
       </c>
       <c r="G25">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H25">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I25">
         <v>0</v>
@@ -2173,33 +2265,36 @@
         <v>0</v>
       </c>
       <c r="O25">
-        <v>2</v>
-      </c>
-      <c r="P25">
-        <v>2</v>
-      </c>
-      <c r="Q25" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.6">
+        <v>1</v>
+      </c>
+      <c r="Q25">
+        <v>0</v>
+      </c>
+      <c r="R25">
+        <v>2</v>
+      </c>
+      <c r="S25" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B26">
         <v>1</v>
       </c>
       <c r="C26">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D26" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F26">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G26">
         <v>0</v>
@@ -2217,7 +2312,7 @@
         <v>0</v>
       </c>
       <c r="L26">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="M26" t="s">
         <v>164</v>
@@ -2226,24 +2321,27 @@
         <v>0</v>
       </c>
       <c r="O26">
-        <v>1</v>
-      </c>
-      <c r="P26">
-        <v>2</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.6">
+        <v>0</v>
+      </c>
+      <c r="Q26">
+        <v>0</v>
+      </c>
+      <c r="R26">
+        <v>2</v>
+      </c>
+      <c r="S26" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C27">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D27" t="s">
         <v>28</v>
@@ -2264,7 +2362,7 @@
         <v>1</v>
       </c>
       <c r="J27">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K27">
         <v>0</v>
@@ -2281,25 +2379,28 @@
       <c r="O27">
         <v>1</v>
       </c>
-      <c r="P27">
-        <v>2</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.6">
+      <c r="Q27">
+        <v>0</v>
+      </c>
+      <c r="R27">
+        <v>2</v>
+      </c>
+      <c r="S27" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="B28">
         <v>2</v>
       </c>
       <c r="C28">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D28" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="E28">
         <v>0</v>
@@ -2311,13 +2412,13 @@
         <v>0</v>
       </c>
       <c r="H28">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J28">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K28">
         <v>0</v>
@@ -2332,16 +2433,19 @@
         <v>0</v>
       </c>
       <c r="O28">
-        <v>1</v>
-      </c>
-      <c r="P28">
-        <v>2</v>
-      </c>
-      <c r="Q28" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.6">
+        <v>2</v>
+      </c>
+      <c r="Q28">
+        <v>0</v>
+      </c>
+      <c r="R28">
+        <v>2</v>
+      </c>
+      <c r="S28" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>74</v>
       </c>
@@ -2387,14 +2491,17 @@
       <c r="O29">
         <v>1</v>
       </c>
-      <c r="P29">
-        <v>2</v>
-      </c>
-      <c r="Q29" t="s">
+      <c r="Q29">
+        <v>0</v>
+      </c>
+      <c r="R29">
+        <v>2</v>
+      </c>
+      <c r="S29" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.6">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>76</v>
       </c>
@@ -2440,25 +2547,28 @@
       <c r="O30">
         <v>2</v>
       </c>
-      <c r="P30">
-        <v>2</v>
-      </c>
-      <c r="Q30" t="s">
+      <c r="Q30">
+        <v>18</v>
+      </c>
+      <c r="R30">
+        <v>2</v>
+      </c>
+      <c r="S30" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.6">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="B31">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C31">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D31" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="E31">
         <v>0</v>
@@ -2467,16 +2577,16 @@
         <v>0</v>
       </c>
       <c r="G31">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I31">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J31">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K31">
         <v>0</v>
@@ -2491,27 +2601,30 @@
         <v>0</v>
       </c>
       <c r="O31">
-        <v>1</v>
-      </c>
-      <c r="P31">
-        <v>2</v>
-      </c>
-      <c r="Q31" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.6">
+        <v>0</v>
+      </c>
+      <c r="Q31">
+        <v>0</v>
+      </c>
+      <c r="R31">
+        <v>2</v>
+      </c>
+      <c r="S31" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B32">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C32">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D32" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="E32">
         <v>0</v>
@@ -2520,16 +2633,16 @@
         <v>0</v>
       </c>
       <c r="G32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H32">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I32">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J32">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K32">
         <v>0</v>
@@ -2546,22 +2659,28 @@
       <c r="O32">
         <v>1</v>
       </c>
-      <c r="P32">
-        <v>2</v>
-      </c>
-      <c r="Q32" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.6">
+      <c r="P32" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q32">
+        <v>42</v>
+      </c>
+      <c r="R32">
+        <v>2</v>
+      </c>
+      <c r="S32" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B33">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C33">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D33" t="s">
         <v>50</v>
@@ -2573,7 +2692,7 @@
         <v>0</v>
       </c>
       <c r="G33">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H33">
         <v>2</v>
@@ -2597,24 +2716,27 @@
         <v>0</v>
       </c>
       <c r="O33">
-        <v>2</v>
-      </c>
-      <c r="P33">
-        <v>2</v>
-      </c>
-      <c r="Q33" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.6">
+        <v>1</v>
+      </c>
+      <c r="Q33">
+        <v>27</v>
+      </c>
+      <c r="R33">
+        <v>2</v>
+      </c>
+      <c r="S33" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B34">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C34">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D34" t="s">
         <v>50</v>
@@ -2626,10 +2748,10 @@
         <v>0</v>
       </c>
       <c r="G34">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H34">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I34">
         <v>0</v>
@@ -2650,39 +2772,42 @@
         <v>0</v>
       </c>
       <c r="O34">
-        <v>0</v>
-      </c>
-      <c r="P34">
-        <v>2</v>
-      </c>
-      <c r="Q34" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.6">
+        <v>2</v>
+      </c>
+      <c r="Q34">
+        <v>0</v>
+      </c>
+      <c r="R34">
+        <v>2</v>
+      </c>
+      <c r="S34" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="B35">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C35">
+        <v>5</v>
+      </c>
+      <c r="D35" t="s">
+        <v>31</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
         <v>3</v>
       </c>
-      <c r="D35" t="s">
-        <v>50</v>
-      </c>
-      <c r="E35">
-        <v>0</v>
-      </c>
-      <c r="F35">
-        <v>0</v>
-      </c>
-      <c r="G35">
-        <v>2</v>
-      </c>
       <c r="H35">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I35">
         <v>0</v>
@@ -2703,24 +2828,27 @@
         <v>0</v>
       </c>
       <c r="O35">
-        <v>1</v>
-      </c>
-      <c r="P35">
-        <v>2</v>
-      </c>
-      <c r="Q35" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.6">
+        <v>2</v>
+      </c>
+      <c r="Q35">
+        <v>0</v>
+      </c>
+      <c r="R35">
+        <v>2</v>
+      </c>
+      <c r="S35" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B36">
         <v>2</v>
       </c>
       <c r="C36">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D36" t="s">
         <v>50</v>
@@ -2732,7 +2860,7 @@
         <v>0</v>
       </c>
       <c r="G36">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H36">
         <v>2</v>
@@ -2756,39 +2884,42 @@
         <v>0</v>
       </c>
       <c r="O36">
-        <v>2</v>
-      </c>
-      <c r="P36">
-        <v>2</v>
-      </c>
-      <c r="Q36" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.6">
+        <v>1</v>
+      </c>
+      <c r="Q36">
+        <v>0</v>
+      </c>
+      <c r="R36">
+        <v>2</v>
+      </c>
+      <c r="S36" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>90</v>
+        <v>62</v>
       </c>
       <c r="B37">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C37">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D37" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="E37">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F37">
         <v>0</v>
       </c>
       <c r="G37">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H37">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I37">
         <v>0</v>
@@ -2809,24 +2940,27 @@
         <v>0</v>
       </c>
       <c r="O37">
-        <v>1</v>
-      </c>
-      <c r="P37">
-        <v>2</v>
-      </c>
-      <c r="Q37" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.6">
+        <v>2</v>
+      </c>
+      <c r="Q37">
+        <v>8</v>
+      </c>
+      <c r="R37">
+        <v>2</v>
+      </c>
+      <c r="S37" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B38">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C38">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D38" t="s">
         <v>28</v>
@@ -2844,7 +2978,7 @@
         <v>0</v>
       </c>
       <c r="I38">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J38">
         <v>1</v>
@@ -2864,16 +2998,19 @@
       <c r="O38">
         <v>1</v>
       </c>
-      <c r="P38">
+      <c r="Q38">
+        <v>0</v>
+      </c>
+      <c r="R38">
         <v>3</v>
       </c>
-      <c r="Q38" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.6">
+      <c r="S38" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="B39">
         <v>1</v>
@@ -2897,10 +3034,10 @@
         <v>0</v>
       </c>
       <c r="I39">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J39">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K39">
         <v>0</v>
@@ -2917,14 +3054,17 @@
       <c r="O39">
         <v>1</v>
       </c>
-      <c r="P39">
+      <c r="Q39">
+        <v>0</v>
+      </c>
+      <c r="R39">
         <v>3</v>
       </c>
-      <c r="Q39" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.6">
+      <c r="S39" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>96</v>
       </c>
@@ -2970,22 +3110,25 @@
       <c r="O40">
         <v>1</v>
       </c>
-      <c r="P40">
+      <c r="Q40">
+        <v>14</v>
+      </c>
+      <c r="R40">
         <v>3</v>
       </c>
-      <c r="Q40" t="s">
+      <c r="S40" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.6">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B41">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C41">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D41" t="s">
         <v>28</v>
@@ -3003,10 +3146,10 @@
         <v>0</v>
       </c>
       <c r="I41">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J41">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K41">
         <v>0</v>
@@ -3021,16 +3164,19 @@
         <v>0</v>
       </c>
       <c r="O41">
-        <v>1</v>
-      </c>
-      <c r="P41">
+        <v>2</v>
+      </c>
+      <c r="Q41">
+        <v>0</v>
+      </c>
+      <c r="R41">
         <v>3</v>
       </c>
-      <c r="Q41" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.6">
+      <c r="S41" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>99</v>
       </c>
@@ -3076,22 +3222,25 @@
       <c r="O42">
         <v>2</v>
       </c>
-      <c r="P42">
+      <c r="Q42">
+        <v>0</v>
+      </c>
+      <c r="R42">
         <v>3</v>
       </c>
-      <c r="Q42" t="s">
+      <c r="S42" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.6">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="B43">
         <v>2</v>
       </c>
       <c r="C43">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D43" t="s">
         <v>28</v>
@@ -3109,10 +3258,10 @@
         <v>0</v>
       </c>
       <c r="I43">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J43">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K43">
         <v>0</v>
@@ -3127,18 +3276,21 @@
         <v>0</v>
       </c>
       <c r="O43">
-        <v>2</v>
-      </c>
-      <c r="P43">
+        <v>1</v>
+      </c>
+      <c r="Q43">
+        <v>0</v>
+      </c>
+      <c r="R43">
         <v>3</v>
       </c>
-      <c r="Q43" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.6">
+      <c r="S43" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>102</v>
+        <v>130</v>
       </c>
       <c r="B44">
         <v>1</v>
@@ -3147,16 +3299,16 @@
         <v>3</v>
       </c>
       <c r="D44" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="E44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H44">
         <v>0</v>
@@ -3168,10 +3320,10 @@
         <v>0</v>
       </c>
       <c r="K44">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="L44">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="M44" t="s">
         <v>166</v>
@@ -3182,34 +3334,37 @@
       <c r="O44">
         <v>0</v>
       </c>
-      <c r="P44">
+      <c r="Q44">
+        <v>0</v>
+      </c>
+      <c r="R44">
         <v>4</v>
       </c>
-      <c r="Q44" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.6">
+      <c r="S44" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B45">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C45">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D45" t="s">
         <v>16</v>
       </c>
       <c r="E45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F45">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H45">
         <v>0</v>
@@ -3233,33 +3388,36 @@
         <v>0</v>
       </c>
       <c r="O45">
-        <v>2</v>
-      </c>
-      <c r="P45">
+        <v>0</v>
+      </c>
+      <c r="Q45">
+        <v>0</v>
+      </c>
+      <c r="R45">
         <v>4</v>
       </c>
-      <c r="Q45" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.6">
+      <c r="S45" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>106</v>
+        <v>132</v>
       </c>
       <c r="B46">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C46">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D46" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="E46">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F46">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G46">
         <v>0</v>
@@ -3274,10 +3432,10 @@
         <v>0</v>
       </c>
       <c r="K46">
-        <v>0</v>
+        <v>-6</v>
       </c>
       <c r="L46">
-        <v>0</v>
+        <v>-6</v>
       </c>
       <c r="M46" t="s">
         <v>166</v>
@@ -3288,28 +3446,34 @@
       <c r="O46">
         <v>1</v>
       </c>
-      <c r="P46">
+      <c r="P46" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q46">
+        <v>39</v>
+      </c>
+      <c r="R46">
         <v>4</v>
       </c>
-      <c r="Q46" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.6">
+      <c r="S46" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B47">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C47">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D47" t="s">
         <v>16</v>
       </c>
       <c r="E47">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F47">
         <v>2</v>
@@ -3339,33 +3503,36 @@
         <v>0</v>
       </c>
       <c r="O47">
-        <v>1</v>
-      </c>
-      <c r="P47">
+        <v>2</v>
+      </c>
+      <c r="Q47">
+        <v>32</v>
+      </c>
+      <c r="R47">
         <v>4</v>
       </c>
-      <c r="Q47" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.6">
+      <c r="S47" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>110</v>
+        <v>128</v>
       </c>
       <c r="B48">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C48">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D48" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="E48">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F48">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G48">
         <v>0</v>
@@ -3380,10 +3547,10 @@
         <v>0</v>
       </c>
       <c r="K48">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="L48">
-        <v>0</v>
+        <v>-6</v>
       </c>
       <c r="M48" t="s">
         <v>166</v>
@@ -3394,16 +3561,19 @@
       <c r="O48">
         <v>1</v>
       </c>
-      <c r="P48">
+      <c r="Q48">
+        <v>0</v>
+      </c>
+      <c r="R48">
         <v>4</v>
       </c>
-      <c r="Q48" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.6">
+      <c r="S48" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B49">
         <v>1</v>
@@ -3447,31 +3617,34 @@
       <c r="O49">
         <v>1</v>
       </c>
-      <c r="P49">
+      <c r="Q49">
+        <v>0</v>
+      </c>
+      <c r="R49">
         <v>4</v>
       </c>
-      <c r="Q49" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.6">
+      <c r="S49" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C50">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D50" t="s">
         <v>16</v>
       </c>
       <c r="E50">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F50">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G50">
         <v>0</v>
@@ -3498,33 +3671,36 @@
         <v>0</v>
       </c>
       <c r="O50">
-        <v>2</v>
-      </c>
-      <c r="P50">
+        <v>1</v>
+      </c>
+      <c r="Q50">
+        <v>0</v>
+      </c>
+      <c r="R50">
         <v>4</v>
       </c>
-      <c r="Q50" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.6">
+      <c r="S50" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B51">
         <v>2</v>
       </c>
       <c r="C51">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D51" t="s">
         <v>16</v>
       </c>
       <c r="E51">
+        <v>0</v>
+      </c>
+      <c r="F51">
         <v>3</v>
-      </c>
-      <c r="F51">
-        <v>2</v>
       </c>
       <c r="G51">
         <v>0</v>
@@ -3551,36 +3727,39 @@
         <v>0</v>
       </c>
       <c r="O51">
-        <v>1</v>
-      </c>
-      <c r="P51">
+        <v>2</v>
+      </c>
+      <c r="Q51">
+        <v>16</v>
+      </c>
+      <c r="R51">
         <v>4</v>
       </c>
-      <c r="Q51" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.6">
+      <c r="S51" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B52">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C52">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D52" t="s">
         <v>16</v>
       </c>
       <c r="E52">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F52">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G52">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H52">
         <v>0</v>
@@ -3606,28 +3785,31 @@
       <c r="O52">
         <v>1</v>
       </c>
-      <c r="P52">
+      <c r="Q52">
+        <v>0</v>
+      </c>
+      <c r="R52">
         <v>4</v>
       </c>
-      <c r="Q52" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.6">
+      <c r="S52" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="B53">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C53">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D53" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="E53">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F53">
         <v>0</v>
@@ -3648,7 +3830,7 @@
         <v>0</v>
       </c>
       <c r="L53">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="M53" t="s">
         <v>166</v>
@@ -3659,31 +3841,34 @@
       <c r="O53">
         <v>2</v>
       </c>
-      <c r="P53">
+      <c r="Q53">
+        <v>25</v>
+      </c>
+      <c r="R53">
         <v>4</v>
       </c>
-      <c r="Q53" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.6">
+      <c r="S53" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B54">
         <v>2</v>
       </c>
       <c r="C54">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D54" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="E54">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F54">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G54">
         <v>0</v>
@@ -3701,7 +3886,7 @@
         <v>0</v>
       </c>
       <c r="L54">
-        <v>-4</v>
+        <v>0</v>
       </c>
       <c r="M54" t="s">
         <v>166</v>
@@ -3710,36 +3895,39 @@
         <v>0</v>
       </c>
       <c r="O54">
-        <v>2</v>
-      </c>
-      <c r="P54">
+        <v>1</v>
+      </c>
+      <c r="Q54">
+        <v>36</v>
+      </c>
+      <c r="R54">
         <v>4</v>
       </c>
-      <c r="Q54" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.6">
+      <c r="S54" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="B55">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C55">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D55" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="E55">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F55">
         <v>0</v>
       </c>
       <c r="G55">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H55">
         <v>0</v>
@@ -3754,7 +3942,7 @@
         <v>0</v>
       </c>
       <c r="L55">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="M55" t="s">
         <v>166</v>
@@ -3763,30 +3951,33 @@
         <v>0</v>
       </c>
       <c r="O55">
-        <v>0</v>
-      </c>
-      <c r="P55">
+        <v>1</v>
+      </c>
+      <c r="Q55">
+        <v>20</v>
+      </c>
+      <c r="R55">
         <v>4</v>
       </c>
-      <c r="Q55" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.6">
+      <c r="S55" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="B56">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C56">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D56" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="E56">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F56">
         <v>0</v>
@@ -3807,7 +3998,7 @@
         <v>0</v>
       </c>
       <c r="L56">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="M56" t="s">
         <v>166</v>
@@ -3818,31 +4009,34 @@
       <c r="O56">
         <v>2</v>
       </c>
-      <c r="P56">
+      <c r="Q56">
+        <v>0</v>
+      </c>
+      <c r="R56">
         <v>4</v>
       </c>
-      <c r="Q56" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.6">
+      <c r="S56" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
       <c r="B57">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C57">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D57" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="E57">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F57">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G57">
         <v>0</v>
@@ -3857,10 +4051,10 @@
         <v>0</v>
       </c>
       <c r="K57">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="L57">
-        <v>-6</v>
+        <v>0</v>
       </c>
       <c r="M57" t="s">
         <v>166</v>
@@ -3871,22 +4065,25 @@
       <c r="O57">
         <v>1</v>
       </c>
-      <c r="P57">
+      <c r="Q57">
+        <v>0</v>
+      </c>
+      <c r="R57">
         <v>4</v>
       </c>
-      <c r="Q57" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.6">
+      <c r="S57" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="B58">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C58">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D58" t="s">
         <v>31</v>
@@ -3910,10 +4107,10 @@
         <v>0</v>
       </c>
       <c r="K58">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="L58">
-        <v>-2</v>
+        <v>-4</v>
       </c>
       <c r="M58" t="s">
         <v>166</v>
@@ -3922,24 +4119,27 @@
         <v>0</v>
       </c>
       <c r="O58">
-        <v>0</v>
-      </c>
-      <c r="P58">
+        <v>2</v>
+      </c>
+      <c r="Q58">
+        <v>0</v>
+      </c>
+      <c r="R58">
         <v>4</v>
       </c>
-      <c r="Q58" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.6">
+      <c r="S58" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="B59">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C59">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D59" t="s">
         <v>31</v>
@@ -3963,10 +4163,10 @@
         <v>0</v>
       </c>
       <c r="K59">
-        <v>-6</v>
+        <v>0</v>
       </c>
       <c r="L59">
-        <v>-6</v>
+        <v>-2</v>
       </c>
       <c r="M59" t="s">
         <v>166</v>
@@ -3975,16 +4175,19 @@
         <v>0</v>
       </c>
       <c r="O59">
-        <v>1</v>
-      </c>
-      <c r="P59">
+        <v>0</v>
+      </c>
+      <c r="Q59">
+        <v>0</v>
+      </c>
+      <c r="R59">
         <v>4</v>
       </c>
-      <c r="Q59" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.6">
+      <c r="S59" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>135</v>
       </c>
@@ -4030,14 +4233,17 @@
       <c r="O60">
         <v>0</v>
       </c>
-      <c r="P60">
+      <c r="Q60">
+        <v>0</v>
+      </c>
+      <c r="R60">
         <v>5</v>
       </c>
-      <c r="Q60" t="s">
+      <c r="S60" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.6">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>138</v>
       </c>
@@ -4083,14 +4289,20 @@
       <c r="O61">
         <v>0</v>
       </c>
-      <c r="P61">
+      <c r="P61" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q61">
+        <v>43</v>
+      </c>
+      <c r="R61">
         <v>5</v>
       </c>
-      <c r="Q61" t="s">
+      <c r="S61" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.6">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>140</v>
       </c>
@@ -4136,14 +4348,17 @@
       <c r="O62">
         <v>0</v>
       </c>
-      <c r="P62">
+      <c r="Q62">
+        <v>0</v>
+      </c>
+      <c r="R62">
         <v>5</v>
       </c>
-      <c r="Q62" t="s">
+      <c r="S62" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.6">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>142</v>
       </c>
@@ -4189,14 +4404,17 @@
       <c r="O63">
         <v>0</v>
       </c>
-      <c r="P63">
+      <c r="Q63">
+        <v>0</v>
+      </c>
+      <c r="R63">
         <v>5</v>
       </c>
-      <c r="Q63" t="s">
+      <c r="S63" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.6">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>144</v>
       </c>
@@ -4242,14 +4460,17 @@
       <c r="O64">
         <v>0</v>
       </c>
-      <c r="P64">
+      <c r="Q64">
         <v>5</v>
       </c>
-      <c r="Q64" t="s">
+      <c r="R64">
+        <v>5</v>
+      </c>
+      <c r="S64" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.6">
+    <row r="65" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>146</v>
       </c>
@@ -4295,14 +4516,17 @@
       <c r="O65">
         <v>0</v>
       </c>
-      <c r="P65">
+      <c r="Q65">
+        <v>0</v>
+      </c>
+      <c r="R65">
         <v>5</v>
       </c>
-      <c r="Q65" t="s">
+      <c r="S65" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.6">
+    <row r="66" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>148</v>
       </c>
@@ -4348,14 +4572,17 @@
       <c r="O66">
         <v>0</v>
       </c>
-      <c r="P66">
+      <c r="Q66">
+        <v>33</v>
+      </c>
+      <c r="R66">
         <v>6</v>
       </c>
-      <c r="Q66" t="s">
+      <c r="S66" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.6">
+    <row r="67" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>150</v>
       </c>
@@ -4401,14 +4628,17 @@
       <c r="O67">
         <v>0</v>
       </c>
-      <c r="P67">
+      <c r="Q67">
+        <v>15</v>
+      </c>
+      <c r="R67">
         <v>6</v>
       </c>
-      <c r="Q67" t="s">
+      <c r="S67" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.6">
+    <row r="68" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>152</v>
       </c>
@@ -4454,14 +4684,17 @@
       <c r="O68">
         <v>0</v>
       </c>
-      <c r="P68">
+      <c r="Q68">
+        <v>23</v>
+      </c>
+      <c r="R68">
         <v>6</v>
       </c>
-      <c r="Q68" t="s">
+      <c r="S68" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.6">
+    <row r="69" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>154</v>
       </c>
@@ -4507,14 +4740,17 @@
       <c r="O69">
         <v>0</v>
       </c>
-      <c r="P69">
+      <c r="Q69">
+        <v>35</v>
+      </c>
+      <c r="R69">
         <v>6</v>
       </c>
-      <c r="Q69" t="s">
+      <c r="S69" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.6">
+    <row r="70" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>156</v>
       </c>
@@ -4560,16 +4796,19 @@
       <c r="O70">
         <v>0</v>
       </c>
-      <c r="P70">
+      <c r="Q70">
+        <v>38</v>
+      </c>
+      <c r="R70">
         <v>6</v>
       </c>
-      <c r="Q70" t="s">
+      <c r="S70" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.6">
+    <row r="71" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B71">
         <v>0</v>
@@ -4578,13 +4817,13 @@
         <v>6</v>
       </c>
       <c r="D71" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="E71">
         <v>0</v>
       </c>
       <c r="F71">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G71">
         <v>0</v>
@@ -4602,7 +4841,7 @@
         <v>0</v>
       </c>
       <c r="L71">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="M71" t="s">
         <v>149</v>
@@ -4613,16 +4852,19 @@
       <c r="O71">
         <v>0</v>
       </c>
-      <c r="P71">
+      <c r="Q71">
+        <v>31</v>
+      </c>
+      <c r="R71">
         <v>6</v>
       </c>
-      <c r="Q71" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.6">
+      <c r="S71" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="72" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B72">
         <v>0</v>
@@ -4631,13 +4873,13 @@
         <v>6</v>
       </c>
       <c r="D72" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="E72">
         <v>0</v>
       </c>
       <c r="F72">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G72">
         <v>0</v>
@@ -4655,7 +4897,7 @@
         <v>0</v>
       </c>
       <c r="L72">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="M72" t="s">
         <v>149</v>
@@ -4666,14 +4908,17 @@
       <c r="O72">
         <v>0</v>
       </c>
-      <c r="P72">
+      <c r="Q72">
+        <v>34</v>
+      </c>
+      <c r="R72">
         <v>6</v>
       </c>
-      <c r="Q72" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.6">
+      <c r="S72" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="73" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>162</v>
       </c>
@@ -4719,14 +4964,21 @@
       <c r="O73">
         <v>0</v>
       </c>
-      <c r="P73">
+      <c r="Q73">
+        <v>37</v>
+      </c>
+      <c r="R73">
         <v>6</v>
       </c>
-      <c r="Q73" t="s">
+      <c r="S73" t="s">
         <v>163</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:S73">
+    <sortCondition ref="R2:R73"/>
+    <sortCondition ref="A2:A73"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>